<commit_message>
Cosmetic changes. Data of sale in guarantee talon now has comfort view.
</commit_message>
<xml_diff>
--- a/static/guarantee.xlsx
+++ b/static/guarantee.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0CD3E2-945C-4C68-80BA-CA559913DF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7150949B-27D5-4D10-B266-A162B8966436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -586,68 +586,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="4" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -655,11 +655,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" s="4" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -667,33 +667,33 @@
         <v>89180010114</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="9" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" s="9" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" s="4" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="11" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="11" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="11" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" s="11" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
@@ -703,23 +703,23 @@
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
     </row>

</xml_diff>